<commit_message>
added final version most likely
</commit_message>
<xml_diff>
--- a/backend/posts.xlsx
+++ b/backend/posts.xlsx
@@ -1,35 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Github/AIorHuman-Research-Website/backend/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A43C093-8D3E-134D-B35F-FD6D7317D855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -72,7 +52,7 @@
     <t>Regarding the Jay Z case and his efforts to silence my clients: Mr. Carter previously denied being the one who sued me and my firm. He filed his frivolous case under a pseudonym. What he fails to say in his recent statement is my firm sent his lawyer a demand letter on behalf of an alleged victim and that victim never demanded a penny from him. Instead, she only sought a confidential mediation. Since I sent the letter on her behalf, Mr. Carter has not only sued me, but he has tried to bully and harass me and this plaintiff. His conduct has had the opposite impact. She is emboldened. I’m very proud of her resolve.  As far as the allegations in the complaint filed, we will let the filing speak for itself and will litigate the facts in court, not in the media.</t>
   </si>
   <si>
-    <t xml:space="preserve">t wasn’t Trump vs. Harris. It was Trump vs. Legacy Media. It was Trump vs. Hollywood. It was Trump vs. Google. It was Trump vs. ChatGPT. It was Trump vs. Tyranny. It was Trump vs. Evil. It was Trump vs. Puppets. It was Trump vs. the Machine. And still, Trump won! </t>
+    <t xml:space="preserve">It wasn’t Trump vs. Harris. It was Trump vs. Legacy Media. It was Trump vs. Hollywood. It was Trump vs. Google. It was Trump vs. ChatGPT. It was Trump vs. Tyranny. It was Trump vs. Evil. It was Trump vs. Puppets. It was Trump vs. the Machine. And still, Trump won! </t>
   </si>
   <si>
     <t>well, God did save his life. He has a little help with WE THE Ppl believed they &amp; fought had lawyers at every voting place. It was amazing Elon in P.A. for 2 wks giving away million dollars every night ! 🇺🇸America fought hard for who they believed   Christians,, NRA, Truckers an amazing the youth and young adults kicked ass, but it was the people that got out that showed you their value and trump went to places no president ever did before. It was an amazing fight. I watched it all from my bedside because I’m bedridden right now I went to every rally on my TV and saw it all happened and watched YMCA became hit the pride. You watched it grow overnight and it was thrilling. It was the most exciting time. The most terrifying time our country has ever faced. I’m so proud of America the real Americans, President, Trump and Elon and all of We the People All voted and got people to the voting and registered him to vote. We fought like it was our last chance to survive and it was, and we did win. Now we have to finish the fight and get Joe Biden paralyzed in his will to destroy the country before he leaves office, he hast to be systematically paralyzed in his ability to utilize money. How can he spend money if Congress doesn’t agree, and if Congress is agreeing, that’s who trump has to work with and thats effing crazy  !!!  America is in big trouble. The real Americans love our country! fought now we have to protect the last 30-40 days because he’s destroying our country! There’s got to be in the constitution a description how to take down the tyrant and a  pure traitor! he hast to be paralyzed in actions and ability to do anything till he leaves office because every day in office he’s trying to more children or tortured and raped and traded to women tortured and raped and men is crazy and all our money is being given away to countries when we need it so bad people are still dying in North Carolina and also bodies missing in states around North Carolina! it’s a nightmare in North Carolina. It’s a war and yeah, our president is destroying our country while eating other countries that there has to be a lot against president leaving Office that’s acting like a tyrant to our own country.</t>
@@ -84,7 +64,7 @@
     <t>Indeed. And he didn’t just win, he won BIGLY. America spoke with one unified voice behind a man who embodies everything America represents — courage, valor, the desire to be the very best in all that we do, the perseverance to get knocked down over and over and over again and still get up and FIGHT…</t>
   </si>
   <si>
-    <t>ust appointed another whackadoodle to the cabinet of whackadoodles! Conspiracy theories, deep state MAGA maggots unite! We can all see thru the BS that MAGA &amp; Project 2025 bring! It's like kindergartners are running the show! Great said nobody ever!</t>
+    <t>Just appointed another whackadoodle to the cabinet of whackadoodles! Conspiracy theories, deep state MAGA maggots unite! We can all see thru the BS that MAGA &amp; Project 2025 bring! It's like kindergartners are running the show! Great said nobody ever!</t>
   </si>
   <si>
     <t>Instead of fighting against so many things, why don’t you fight for a Americans. Why don’t you sit down with your Republican encounter parts and do what’s good for the people? Things like bring jobs back to the United States, reduce crime, reduce the national debt, stop the illegal flow of immigrants into this country. Do better.</t>
@@ -130,7 +110,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF1D9BF0"/>
+        <color rgb="FF1d9bf0"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
       </rPr>
@@ -148,7 +128,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF1D9BF0"/>
+        <color rgb="FF1d9bf0"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
       </rPr>
@@ -292,7 +272,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -304,8 +284,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,26 +296,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF1D9BF0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
@@ -342,7 +305,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -372,55 +334,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="20">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -431,10 +412,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -472,71 +453,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -564,7 +545,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -587,11 +568,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -600,13 +581,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -616,7 +597,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -625,7 +606,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -634,7 +615,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -642,10 +623,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -710,57 +691,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="16" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="51.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="18" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="18" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="18" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="19" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="31.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="4"/>
       <c r="I1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="168" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="185.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="7">
@@ -778,12 +767,18 @@
       <c r="G2" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="121.5">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="7">
@@ -801,12 +796,18 @@
       <c r="G3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="147">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7">
@@ -824,23 +825,39 @@
       <c r="G4" s="7">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="185.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="185.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="63.75">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
@@ -858,12 +875,18 @@
       <c r="G6" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="409.5">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="7">
@@ -881,17 +904,24 @@
       <c r="G7" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="75">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
+      <c r="D8" s="9"/>
       <c r="E8" s="7">
         <v>0</v>
       </c>
@@ -901,17 +931,24 @@
       <c r="G8" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="75">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
       </c>
+      <c r="D9" s="9"/>
       <c r="E9" s="7">
         <v>0</v>
       </c>
@@ -921,17 +958,24 @@
       <c r="G9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="63.75">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
       </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="7">
         <v>0</v>
       </c>
@@ -941,17 +985,24 @@
       <c r="G10" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="75">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
       </c>
+      <c r="D11" s="9"/>
       <c r="E11" s="7">
         <v>0</v>
       </c>
@@ -961,12 +1012,18 @@
       <c r="G11" s="7">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="121.5">
+      <c r="A12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="7">
@@ -984,17 +1041,24 @@
       <c r="G12" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="63.75">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="7">
         <v>0</v>
       </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="7">
         <v>0</v>
       </c>
@@ -1004,17 +1068,24 @@
       <c r="G13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="76.5">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="7">
         <v>2</v>
       </c>
+      <c r="D14" s="9"/>
       <c r="E14" s="7">
         <v>0</v>
       </c>
@@ -1024,17 +1095,24 @@
       <c r="G14" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="87">
+      <c r="A15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="7">
         <v>0</v>
       </c>
@@ -1044,17 +1122,24 @@
       <c r="G15" s="7">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="75">
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
       </c>
+      <c r="D16" s="9"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -1064,17 +1149,24 @@
       <c r="G16" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="49">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
       </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="7">
         <v>0</v>
       </c>
@@ -1084,12 +1176,18 @@
       <c r="G17" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="7">
@@ -1107,17 +1205,24 @@
       <c r="G18" s="7">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="7">
         <v>7</v>
       </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="7">
         <v>0</v>
       </c>
@@ -1127,12 +1232,18 @@
       <c r="G19" s="7">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="H19" s="8"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="7">
@@ -1150,17 +1261,24 @@
       <c r="G20" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="7">
         <v>62</v>
       </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="7">
         <v>0</v>
       </c>
@@ -1170,17 +1288,24 @@
       <c r="G21" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+      <c r="A22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
+      <c r="D22" s="9"/>
       <c r="E22" s="7">
         <v>0</v>
       </c>
@@ -1190,12 +1315,18 @@
       <c r="G22" s="7">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+      <c r="A23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="7">
@@ -1213,17 +1344,24 @@
       <c r="G23" s="7">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+      <c r="A24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="7">
         <v>2</v>
       </c>
+      <c r="D24" s="9"/>
       <c r="E24" s="7">
         <v>0</v>
       </c>
@@ -1233,17 +1371,24 @@
       <c r="G24" s="7">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="H24" s="8"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+      <c r="A25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="7">
         <v>0</v>
       </c>
@@ -1253,17 +1398,24 @@
       <c r="G25" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+      <c r="A26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="7">
         <v>1</v>
       </c>
+      <c r="D26" s="9"/>
       <c r="E26" s="7">
         <v>0</v>
       </c>
@@ -1273,12 +1425,18 @@
       <c r="G26" s="7">
         <v>68</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="7">
@@ -1296,12 +1454,18 @@
       <c r="G27" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+      <c r="A28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="7">
@@ -1319,17 +1483,24 @@
       <c r="G28" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="H28" s="8"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+      <c r="A29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="7">
         <v>7</v>
       </c>
+      <c r="D29" s="9"/>
       <c r="E29" s="7">
         <v>0</v>
       </c>
@@ -1339,23 +1510,39 @@
       <c r="G29" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+      <c r="A30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C30" s="9"/>
       <c r="D30" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="5"/>
@@ -1363,59 +1550,87 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
+      <c r="H31" s="4"/>
       <c r="I31" s="5"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+      <c r="A32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L32" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8" t="s">
         <v>39</v>
       </c>
       <c r="M32" s="7">
         <f>COUNTIF(C:G, "&gt;50")/5</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+      <c r="A33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L33" t="s">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="12">
         <f>COUNTIF(C:G,"&lt;50")/5</f>
-        <v>22.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+      <c r="A34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L34" t="s">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="12">
         <f>M32 / (M32+M33)</f>
-        <v>0.3105590062111801</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="5"/>
@@ -1423,14 +1638,18 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
+      <c r="H35" s="4"/>
       <c r="I35" s="5"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="5"/>
@@ -1438,14 +1657,18 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
       <c r="I36" s="5"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="5"/>
@@ -1453,14 +1676,18 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
+      <c r="H37" s="4"/>
       <c r="I37" s="5"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C38" s="5"/>
@@ -1468,29 +1695,41 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
+      <c r="H38" s="4"/>
       <c r="I38" s="5"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+      <c r="A39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H39" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="8" t="s">
         <v>49</v>
       </c>
       <c r="I39" s="7">
         <f>COUNTIF(B:B, "*")</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="3" t="s">
+      </c>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="5"/>
@@ -1498,14 +1737,18 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
+      <c r="H40" s="4"/>
       <c r="I40" s="5"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C41" s="5"/>
@@ -1513,11 +1756,15 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="I41" s="11"/>
-      <c r="M41" s="12"/>
-    </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="H41" s="4"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25" customFormat="1" s="1">
+      <c r="A42" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1538,188 +1785,255 @@
       <c r="G42" s="5">
         <v>100</v>
       </c>
+      <c r="H42" s="4"/>
       <c r="I42" s="5"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+      <c r="A43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="13">
-        <v>100</v>
-      </c>
-      <c r="D43" s="13">
-        <v>100</v>
-      </c>
-      <c r="E43" s="13">
-        <v>100</v>
-      </c>
-      <c r="F43" s="13">
-        <v>100</v>
-      </c>
-      <c r="G43" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C43" s="7">
+        <v>100</v>
+      </c>
+      <c r="D43" s="7">
+        <v>100</v>
+      </c>
+      <c r="E43" s="7">
+        <v>100</v>
+      </c>
+      <c r="F43" s="7">
+        <v>100</v>
+      </c>
+      <c r="G43" s="7">
+        <v>100</v>
+      </c>
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+      <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="13">
-        <v>100</v>
-      </c>
-      <c r="D44" s="13">
-        <v>100</v>
-      </c>
-      <c r="E44" s="13">
-        <v>100</v>
-      </c>
-      <c r="F44" s="13">
-        <v>100</v>
-      </c>
-      <c r="G44" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="C44" s="7">
+        <v>100</v>
+      </c>
+      <c r="D44" s="7">
+        <v>100</v>
+      </c>
+      <c r="E44" s="7">
+        <v>100</v>
+      </c>
+      <c r="F44" s="7">
+        <v>100</v>
+      </c>
+      <c r="G44" s="7">
+        <v>100</v>
+      </c>
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+      <c r="A45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="13">
-        <v>100</v>
-      </c>
-      <c r="D45" s="13">
-        <v>100</v>
-      </c>
-      <c r="E45" s="13">
-        <v>100</v>
-      </c>
-      <c r="F45" s="13">
-        <v>100</v>
-      </c>
-      <c r="G45" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="C45" s="7">
+        <v>100</v>
+      </c>
+      <c r="D45" s="7">
+        <v>100</v>
+      </c>
+      <c r="E45" s="7">
+        <v>100</v>
+      </c>
+      <c r="F45" s="7">
+        <v>100</v>
+      </c>
+      <c r="G45" s="7">
+        <v>100</v>
+      </c>
+      <c r="H45" s="8"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+      <c r="A46" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="13">
-        <v>100</v>
-      </c>
-      <c r="D46" s="13">
-        <v>100</v>
-      </c>
-      <c r="E46" s="13">
-        <v>100</v>
-      </c>
-      <c r="F46" s="13">
-        <v>100</v>
-      </c>
-      <c r="G46" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="C46" s="7">
+        <v>100</v>
+      </c>
+      <c r="D46" s="7">
+        <v>100</v>
+      </c>
+      <c r="E46" s="7">
+        <v>100</v>
+      </c>
+      <c r="F46" s="7">
+        <v>100</v>
+      </c>
+      <c r="G46" s="7">
+        <v>100</v>
+      </c>
+      <c r="H46" s="8"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+      <c r="A47" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="13">
-        <v>100</v>
-      </c>
-      <c r="D47" s="13">
-        <v>100</v>
-      </c>
-      <c r="E47" s="13">
-        <v>100</v>
-      </c>
-      <c r="F47" s="13">
-        <v>100</v>
-      </c>
-      <c r="G47" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="C47" s="7">
+        <v>100</v>
+      </c>
+      <c r="D47" s="7">
+        <v>100</v>
+      </c>
+      <c r="E47" s="7">
+        <v>100</v>
+      </c>
+      <c r="F47" s="7">
+        <v>100</v>
+      </c>
+      <c r="G47" s="7">
+        <v>100</v>
+      </c>
+      <c r="H47" s="8"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+      <c r="A48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="8">
-        <v>0</v>
-      </c>
-      <c r="E48" s="8">
-        <v>0</v>
-      </c>
-      <c r="F48" s="8">
-        <v>0</v>
-      </c>
-      <c r="G48" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C48" s="15">
+        <v>0</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="15">
+        <v>0</v>
+      </c>
+      <c r="F48" s="15">
+        <v>0</v>
+      </c>
+      <c r="G48" s="15">
+        <v>0</v>
+      </c>
+      <c r="H48" s="8"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+      <c r="A49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="15">
         <v>2</v>
       </c>
-      <c r="E49" s="8">
-        <v>0</v>
-      </c>
-      <c r="F49" s="8">
-        <v>0</v>
-      </c>
-      <c r="G49" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="D49" s="9"/>
+      <c r="E49" s="15">
+        <v>0</v>
+      </c>
+      <c r="F49" s="15">
+        <v>0</v>
+      </c>
+      <c r="G49" s="15">
+        <v>0</v>
+      </c>
+      <c r="H49" s="8"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+      <c r="A50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="15">
         <v>6</v>
       </c>
-      <c r="E50" s="8">
+      <c r="D50" s="9"/>
+      <c r="E50" s="15">
         <v>23</v>
       </c>
-      <c r="F50" s="8">
-        <v>0</v>
-      </c>
-      <c r="G50" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>7</v>
-      </c>
+      <c r="F50" s="15">
+        <v>0</v>
+      </c>
+      <c r="G50" s="15">
+        <v>0</v>
+      </c>
+      <c r="H50" s="8"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+      <c r="A51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>